<commit_message>
fixed problem in library sheet 01.06.19
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_fullrun_hbrown_01.30.20.xlsx
+++ b/fastqFiles/fastq_fullrun_hbrown_01.30.20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB94B949-4790-3E4A-BEC7-C1D10DEA98DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0765B23-19D0-3B4B-A32E-DA6913B21AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33220" windowHeight="13920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="33">
   <si>
     <t>libraryDate</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>01.06.20</t>
+  </si>
+  <si>
+    <t>01.16.20</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1005,7 +1008,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
@@ -1042,7 +1045,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -1080,7 +1083,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
@@ -1117,7 +1120,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
@@ -1155,7 +1158,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
fixing problems with library 01.06.20 and library 01.16.20
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_fullrun_hbrown_01.30.20.xlsx
+++ b/fastqFiles/fastq_fullrun_hbrown_01.30.20.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0765B23-19D0-3B4B-A32E-DA6913B21AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93BBC98-940C-AA41-B0FD-4C4BA555BFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33220" windowHeight="13920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="2280" windowWidth="33220" windowHeight="13920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="59">
   <si>
     <t>libraryDate</t>
   </si>
@@ -120,17 +120,95 @@
     <t>Brent_JR310_GTAC_57_SIC_Index2_07_CGAAAGT_GAGTTGGT_S43_R1_001.fastq.gz</t>
   </si>
   <si>
-    <t>01.06.20</t>
-  </si>
-  <si>
     <t>01.16.20</t>
+  </si>
+  <si>
+    <t>Brent_5c1_GTAC_1_SIC_Index2_06_TGAGGTT_GACCTTGT_S2_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c2_GTAC_2_SIC_Index2_06_GCTTAGA_GACCTTGT_S3_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c3_GTAC_3_SIC_Index2_06_ATGACAG_GACCTTGT_S4_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c4_GTAC_4_SIC_Index2_06_CACCTCC_GACCTTGT_S5_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c5_GTAC_5_SIC_Index2_06_ATCGAGC_GACCTTGT_S6_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c6_GTAC_6_SIC_Index2_06_TACTCTA_GACCTTGT_S7_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c7_GTAC_7_SIC_Index2_06_AGACTGA_GACCTTGT_S8_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c8_GTAC_8_SIC_Index2_06_CTTGGAA_GACCTTGT_S9_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c9_GTAC_9_SIC_Index2_06_CCGATTA_GACCTTGT_S10_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c10_GTAC_10_SIC_Index2_06_GGCAGCG_GACCTTGT_S11_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c11_GTAC_11_SIC_Index2_06_CCATCAT_GACCTTGT_S12_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c12_GTAC_12_SIC_Index2_06_TAACAAG_GACCTTGT_S13_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c13_GTAC_13_SIC_Index2_06_GAGGCGT_GACCTTGT_S14_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c14_GTAC_14_SIC_Index2_06_TTTAACT_GACCTTGT_S15_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c15_GTAC_15_SIC_Index2_06_GGTCCTC_GACCTTGT_S16_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c16_GTAC_16_SIC_Index2_06_CGGTGGC_GACCTTGT_S17_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c17_GTAC_17_SIC_Index2_06_ACTGTCG_GACCTTGT_S18_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c18_GTAC_18_SIC_Index2_06_GTATTTG_GACCTTGT_S19_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c19_GTAC_19_SIC_Index2_06_GAGTACG_GACCTTGT_S20_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c20_GTAC_20_SIC_Index2_06_ACAGATA_GACCTTGT_S21_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c21_GTAC_21_SIC_Index2_06_CTCAATG_GACCTTGT_S22_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c22_GTAC_22_SIC_Index2_06_AAATGCA_GACCTTGT_S23_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c23_GTAC_23_SIC_Index2_06_ACGCGGG_GACCTTGT_S24_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c24_GTAC_24_SIC_Index2_06_GGAGTCC_GACCTTGT_S25_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c25_GTAC_25_SIC_Index2_06_CGTCGCT_GACCTTGT_S26_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_5c26_GTAC_26_SIC_Index2_06_TCAACTG_GACCTTGT_S27_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>01.10.20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -172,6 +250,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -211,6 +295,8 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1008,7 +1094,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
@@ -1045,7 +1131,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -1083,7 +1169,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
@@ -1120,7 +1206,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
@@ -1158,7 +1244,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
@@ -1192,6 +1278,916 @@
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <v>41.8</v>
+      </c>
+      <c r="I18">
+        <v>0.94373419367483169</v>
+      </c>
+      <c r="J18" s="12">
+        <v>11295855</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19">
+        <v>16.8</v>
+      </c>
+      <c r="I19">
+        <v>0.7779716205845526</v>
+      </c>
+      <c r="J19" s="12">
+        <v>14320290</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20">
+        <v>44</v>
+      </c>
+      <c r="I20">
+        <v>0.96642685388531446</v>
+      </c>
+      <c r="J20" s="12">
+        <v>14577668</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="I21">
+        <v>0.78249857027228897</v>
+      </c>
+      <c r="J21" s="12">
+        <v>12115310</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22">
+        <v>69</v>
+      </c>
+      <c r="I22">
+        <v>0.91470253011960168</v>
+      </c>
+      <c r="J22" s="12">
+        <v>10841856</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23">
+        <v>17</v>
+      </c>
+      <c r="I23">
+        <v>0.62897359186328961</v>
+      </c>
+      <c r="J23" s="12">
+        <v>12144022</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24">
+        <v>15.2</v>
+      </c>
+      <c r="I24">
+        <v>0.72785343662340307</v>
+      </c>
+      <c r="J24" s="12">
+        <v>13264007</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25">
+        <v>7.01</v>
+      </c>
+      <c r="I25">
+        <v>1.0525063655213405</v>
+      </c>
+      <c r="J25" s="12">
+        <v>13539175</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26">
+        <v>22.9</v>
+      </c>
+      <c r="I26">
+        <v>0.92770260757448897</v>
+      </c>
+      <c r="J26" s="12">
+        <v>10781922</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27">
+        <v>30</v>
+      </c>
+      <c r="I27">
+        <v>1.0524407774172397</v>
+      </c>
+      <c r="J27" s="12">
+        <v>14477043</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="I28">
+        <v>1.0318570686798922</v>
+      </c>
+      <c r="J28" s="12">
+        <v>12194237</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29">
+        <v>28.3</v>
+      </c>
+      <c r="I29">
+        <v>0.7494627292754179</v>
+      </c>
+      <c r="J29" s="12">
+        <v>11389794</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30">
+        <v>23.7</v>
+      </c>
+      <c r="I30">
+        <v>0.76930462487595208</v>
+      </c>
+      <c r="J30" s="12">
+        <v>11789158</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31">
+        <v>15.6</v>
+      </c>
+      <c r="I31">
+        <v>0.71898770161116654</v>
+      </c>
+      <c r="J31" s="12">
+        <v>13067756</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32">
+        <v>46.1</v>
+      </c>
+      <c r="I32">
+        <v>1.1053538871745974</v>
+      </c>
+      <c r="J32" s="12">
+        <v>17567359</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33">
+        <v>11.4</v>
+      </c>
+      <c r="I33">
+        <v>0.75947007783284914</v>
+      </c>
+      <c r="J33" s="12">
+        <v>11545177</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>17</v>
+      </c>
+      <c r="D34" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34">
+        <v>25.8</v>
+      </c>
+      <c r="I34">
+        <v>0.91009457416184469</v>
+      </c>
+      <c r="J34" s="12">
+        <v>10728440</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>18</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35">
+        <v>23.2</v>
+      </c>
+      <c r="I35">
+        <v>0.93678915626590054</v>
+      </c>
+      <c r="J35" s="12">
+        <v>12148062</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>19</v>
+      </c>
+      <c r="D36" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36">
+        <v>25.4</v>
+      </c>
+      <c r="I36">
+        <v>0.95914509419362748</v>
+      </c>
+      <c r="J36" s="12">
+        <v>13880375</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>20</v>
+      </c>
+      <c r="D37" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37">
+        <v>23.3</v>
+      </c>
+      <c r="I37">
+        <v>0.88158612798169178</v>
+      </c>
+      <c r="J37" s="12">
+        <v>13227029</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>21</v>
+      </c>
+      <c r="D38" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="I38">
+        <v>30.293324138598532</v>
+      </c>
+      <c r="J38" s="12">
+        <v>5191510</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>22</v>
+      </c>
+      <c r="D39" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="I39">
+        <v>7.7849649914810541</v>
+      </c>
+      <c r="J39" s="12">
+        <v>13590254</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>23</v>
+      </c>
+      <c r="D40" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>13.52171964272214</v>
+      </c>
+      <c r="J40" s="12">
+        <v>11545393</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>24</v>
+      </c>
+      <c r="D41" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+      <c r="I41">
+        <v>2.9940869793970992</v>
+      </c>
+      <c r="J41" s="12">
+        <v>10242360</v>
+      </c>
+      <c r="K41" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>25</v>
+      </c>
+      <c r="D42" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42">
+        <v>11</v>
+      </c>
+      <c r="I42">
+        <v>0.54330620843577582</v>
+      </c>
+      <c r="J42" s="12">
+        <v>12923568</v>
+      </c>
+      <c r="K42" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>26</v>
+      </c>
+      <c r="D43" s="5">
+        <v>4178</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43">
+        <v>14.9</v>
+      </c>
+      <c r="I43">
+        <v>0.51730888025304267</v>
+      </c>
+      <c r="J43" s="12">
+        <v>15000389</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>